<commit_message>
fix title and icons
</commit_message>
<xml_diff>
--- a/sample/data_1.xlsx
+++ b/sample/data_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5101" uniqueCount="3565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5101" uniqueCount="3568">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -10546,34 +10546,7 @@
     <t xml:space="preserve">https://{s}.tile.opentopomap.org/{z}/{x}/{y}.png</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Map data: &amp;copy; &lt;a href="https://www.openstreetmap.org/copyright"&gt;OpenStreetMap&lt;/a&gt; contributors, &lt;a href="http://viewfinderpanoramas.org"&gt;SRTM&lt;/a&gt; | Map style: &amp;copy; &lt;a href="https://opentopomap.org"&gt;OpenTopoMap&lt;/a&gt; (&lt;a href="</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://creativecommons.org/licenses/by-sa/3.0/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"&gt;CC-BY-SA&lt;/a&gt;)</t>
-    </r>
+    <t xml:space="preserve">Map data: &amp;copy; &lt;a href="https://www.openstreetmap.org/copyright"&gt;OpenStreetMap&lt;/a&gt; contributors, &lt;a href="http://viewfinderpanoramas.org"&gt;SRTM&lt;/a&gt; | Map style: &amp;copy; &lt;a href="https://opentopomap.org"&gt;OpenTopoMap&lt;/a&gt; (&lt;a href="https://creativecommons.org/licenses/by-sa/3.0/"&gt;CC-BY-SA&lt;/a&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">osm</t>
@@ -10699,25 +10672,34 @@
     <t xml:space="preserve">Dyrekcja regionalna</t>
   </si>
   <si>
+    <t xml:space="preserve">building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punkty</t>
+  </si>
+  <si>
     <t xml:space="preserve">circle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Punkty</t>
   </si>
   <si>
     <t xml:space="preserve">black</t>
@@ -11301,9 +11283,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="35.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="65.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="65.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="181.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="18" style="3" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="3" width="11.54"/>
@@ -35356,7 +35338,7 @@
       <c r="F2" s="41" t="n">
         <v>17</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="42" t="s">
         <v>3506</v>
       </c>
       <c r="AMJ2" s="43"/>
@@ -35413,7 +35395,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://creativecommons.org/licenses/by-sa/3.0/"/>
+    <hyperlink ref="G2" r:id="rId1" display="Map data: &amp;copy; &lt;a href=&quot;https://www.openstreetmap.org/copyright&quot;&gt;OpenStreetMap&lt;/a&gt; contributors, &lt;a href=&quot;http://viewfinderpanoramas.org&quot;&gt;SRTM&lt;/a&gt; | Map style: &amp;copy; &lt;a href=&quot;https://opentopomap.org&quot;&gt;OpenTopoMap&lt;/a&gt; (&lt;a href=&quot;https://creativecommons.org/licenses/by-sa/3.0/&quot;&gt;CC-BY-SA&lt;/a&gt;)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -35432,15 +35414,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="32.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="80.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="32.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="80.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="40" width="13.24"/>
@@ -36711,17 +36693,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="46" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.3"/>
@@ -36866,13 +36848,13 @@
         <v>3520</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>3548</v>
+        <v>3550</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>3544</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>3550</v>
+        <v>3551</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>3546</v>
@@ -36892,19 +36874,19 @@
     </row>
     <row r="5" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>3551</v>
+        <v>3552</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>3522</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>3548</v>
+        <v>3553</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>3544</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>3552</v>
+        <v>3554</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>3546</v>
@@ -36924,19 +36906,19 @@
     </row>
     <row r="6" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>3553</v>
+        <v>3555</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>3554</v>
+        <v>3556</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>3548</v>
+        <v>3557</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>3544</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>3555</v>
+        <v>3558</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>3546</v>
@@ -36956,10 +36938,10 @@
     </row>
     <row r="7" s="16" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>3556</v>
+        <v>3559</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>3557</v>
+        <v>3560</v>
       </c>
       <c r="G7" s="51"/>
       <c r="H7" s="16" t="n">
@@ -36969,25 +36951,25 @@
         <v>20</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>3558</v>
+        <v>3561</v>
       </c>
       <c r="L7" s="45" t="s">
-        <v>3559</v>
+        <v>3562</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>3560</v>
+        <v>3563</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>3561</v>
+        <v>3564</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>3562</v>
+        <v>3565</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>3563</v>
+        <v>3566</v>
       </c>
       <c r="Q7" s="16" t="s">
-        <v>3564</v>
+        <v>3567</v>
       </c>
       <c r="AMH7" s="21"/>
       <c r="AMI7" s="21"/>

</xml_diff>